<commit_message>
update water reservoir excel and jupyter notebook
</commit_message>
<xml_diff>
--- a/Examples/ANP_Water_Reservoir/WaterReservior_results_Limit.xlsx
+++ b/Examples/ANP_Water_Reservoir/WaterReservior_results_Limit.xlsx
@@ -420,13 +420,13 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>0.2408311724041815</v>
+        <v>0.3613244253276712</v>
       </c>
       <c r="C2">
-        <v>0.2408311724041815</v>
+        <v>0.3613244253276712</v>
       </c>
       <c r="D2">
-        <v>0.2408311724041816</v>
+        <v>0.3613244253276711</v>
       </c>
       <c r="E2">
         <v>0</v>
@@ -443,13 +443,13 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>0.3742737492009104</v>
+        <v>0.3776126654937615</v>
       </c>
       <c r="C3">
-        <v>0.3742737492009104</v>
+        <v>0.3776126654937615</v>
       </c>
       <c r="D3">
-        <v>0.3742737492009104</v>
+        <v>0.3776126654937615</v>
       </c>
       <c r="E3">
         <v>0</v>
@@ -466,13 +466,13 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>0.384895078394908</v>
+        <v>0.2610629091785673</v>
       </c>
       <c r="C4">
-        <v>0.3848950783949081</v>
+        <v>0.2610629091785673</v>
       </c>
       <c r="D4">
-        <v>0.3848950783949081</v>
+        <v>0.2610629091785673</v>
       </c>
       <c r="E4">
         <v>0</v>
@@ -498,13 +498,13 @@
         <v>0</v>
       </c>
       <c r="E5">
-        <v>0.2231518276835295</v>
+        <v>0.537756771336699</v>
       </c>
       <c r="F5">
-        <v>0.2231518276835295</v>
+        <v>0.537756771336699</v>
       </c>
       <c r="G5">
-        <v>0.2231518276835295</v>
+        <v>0.537756771336699</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -521,13 +521,13 @@
         <v>0</v>
       </c>
       <c r="E6">
-        <v>0.3719475108519568</v>
+        <v>0.2289086716580906</v>
       </c>
       <c r="F6">
-        <v>0.3719475108519568</v>
+        <v>0.2289086716580906</v>
       </c>
       <c r="G6">
-        <v>0.3719475108519568</v>
+        <v>0.2289086716580905</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -544,13 +544,13 @@
         <v>0</v>
       </c>
       <c r="E7">
-        <v>0.4049006614645136</v>
+        <v>0.2333345570052105</v>
       </c>
       <c r="F7">
-        <v>0.4049006614645137</v>
+        <v>0.2333345570052105</v>
       </c>
       <c r="G7">
-        <v>0.4049006614645136</v>
+        <v>0.2333345570052105</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
assign same scale multiple times bug
</commit_message>
<xml_diff>
--- a/Examples/ANP_Water_Reservoir/WaterReservior_results_Limit.xlsx
+++ b/Examples/ANP_Water_Reservoir/WaterReservior_results_Limit.xlsx
@@ -420,13 +420,13 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>0.3613244253276712</v>
+        <v>0.2408311724041815</v>
       </c>
       <c r="C2">
-        <v>0.3613244253276712</v>
+        <v>0.2408311724041815</v>
       </c>
       <c r="D2">
-        <v>0.3613244253276711</v>
+        <v>0.2408311724041816</v>
       </c>
       <c r="E2">
         <v>0</v>
@@ -443,13 +443,13 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>0.3776126654937615</v>
+        <v>0.3742737492009104</v>
       </c>
       <c r="C3">
-        <v>0.3776126654937615</v>
+        <v>0.3742737492009104</v>
       </c>
       <c r="D3">
-        <v>0.3776126654937615</v>
+        <v>0.3742737492009104</v>
       </c>
       <c r="E3">
         <v>0</v>
@@ -466,13 +466,13 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>0.2610629091785673</v>
+        <v>0.384895078394908</v>
       </c>
       <c r="C4">
-        <v>0.2610629091785673</v>
+        <v>0.3848950783949081</v>
       </c>
       <c r="D4">
-        <v>0.2610629091785673</v>
+        <v>0.3848950783949081</v>
       </c>
       <c r="E4">
         <v>0</v>
@@ -498,13 +498,13 @@
         <v>0</v>
       </c>
       <c r="E5">
-        <v>0.537756771336699</v>
+        <v>0.2231518276835295</v>
       </c>
       <c r="F5">
-        <v>0.537756771336699</v>
+        <v>0.2231518276835295</v>
       </c>
       <c r="G5">
-        <v>0.537756771336699</v>
+        <v>0.2231518276835295</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -521,13 +521,13 @@
         <v>0</v>
       </c>
       <c r="E6">
-        <v>0.2289086716580906</v>
+        <v>0.3719475108519568</v>
       </c>
       <c r="F6">
-        <v>0.2289086716580906</v>
+        <v>0.3719475108519568</v>
       </c>
       <c r="G6">
-        <v>0.2289086716580905</v>
+        <v>0.3719475108519568</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -544,13 +544,13 @@
         <v>0</v>
       </c>
       <c r="E7">
-        <v>0.2333345570052105</v>
+        <v>0.4049006614645136</v>
       </c>
       <c r="F7">
-        <v>0.2333345570052105</v>
+        <v>0.4049006614645137</v>
       </c>
       <c r="G7">
-        <v>0.2333345570052105</v>
+        <v>0.4049006614645136</v>
       </c>
     </row>
   </sheetData>

</xml_diff>